<commit_message>
added results for e,s and l duration
</commit_message>
<xml_diff>
--- a/Villa.xlsx
+++ b/Villa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="164">
   <si>
     <t>Task</t>
   </si>
@@ -148,15 +148,15 @@
     <t>I.3</t>
   </si>
   <si>
+    <t>J.2</t>
+  </si>
+  <si>
+    <t>J.3</t>
+  </si>
+  <si>
     <t>J.1</t>
   </si>
   <si>
-    <t>J.2</t>
-  </si>
-  <si>
-    <t>J.3</t>
-  </si>
-  <si>
     <t>K.1</t>
   </si>
   <si>
@@ -292,12 +292,12 @@
     <t>['H.2', 'H.3']</t>
   </si>
   <si>
-    <t>['I.2', 'I.3']</t>
-  </si>
-  <si>
     <t>['I.1', 'I.2', 'I.3']</t>
   </si>
   <si>
+    <t>['J.2', 'J.3']</t>
+  </si>
+  <si>
     <t>['J.1']</t>
   </si>
   <si>
@@ -337,12 +337,6 @@
     <t>['Q.3']</t>
   </si>
   <si>
-    <t>['J.2', 'J.3']</t>
-  </si>
-  <si>
-    <t>['J.1', 'J.2', 'J.3']</t>
-  </si>
-  <si>
     <t>['Completion']</t>
   </si>
   <si>
@@ -430,13 +424,13 @@
     <t>Installation of Fire System</t>
   </si>
   <si>
+    <t>Interior Brick Wall</t>
+  </si>
+  <si>
+    <t>Exterior Brick Wall</t>
+  </si>
+  <si>
     <t>Drywall</t>
-  </si>
-  <si>
-    <t>Interior Brick Wall</t>
-  </si>
-  <si>
-    <t>Exterior Brick Wall</t>
   </si>
   <si>
     <t>Plaster (ext-int)</t>
@@ -950,7 +944,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -982,7 +976,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F4">
         <v>12</v>
@@ -1014,7 +1008,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F5">
         <v>12</v>
@@ -1046,7 +1040,7 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F6">
         <v>12</v>
@@ -1078,7 +1072,7 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F7">
         <v>18</v>
@@ -1110,7 +1104,7 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F8">
         <v>22</v>
@@ -1142,7 +1136,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F9">
         <v>22</v>
@@ -1174,7 +1168,7 @@
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F10">
         <v>22</v>
@@ -1206,7 +1200,7 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F11">
         <v>30</v>
@@ -1238,7 +1232,7 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F12">
         <v>38</v>
@@ -1270,7 +1264,7 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F13">
         <v>38</v>
@@ -1302,7 +1296,7 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F14">
         <v>44</v>
@@ -1334,7 +1328,7 @@
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F15">
         <v>48</v>
@@ -1366,7 +1360,7 @@
         <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F16">
         <v>60</v>
@@ -1398,7 +1392,7 @@
         <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F17">
         <v>80</v>
@@ -1430,7 +1424,7 @@
         <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F18">
         <v>98</v>
@@ -1462,7 +1456,7 @@
         <v>30</v>
       </c>
       <c r="E19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F19">
         <v>98</v>
@@ -1494,7 +1488,7 @@
         <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F20">
         <v>128</v>
@@ -1526,7 +1520,7 @@
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F21">
         <v>144</v>
@@ -1558,7 +1552,7 @@
         <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F22">
         <v>144</v>
@@ -1590,7 +1584,7 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F23">
         <v>144</v>
@@ -1622,7 +1616,7 @@
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F24">
         <v>144</v>
@@ -1654,7 +1648,7 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F25">
         <v>156</v>
@@ -1686,7 +1680,7 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F26">
         <v>164</v>
@@ -1718,7 +1712,7 @@
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F27">
         <v>164</v>
@@ -1750,7 +1744,7 @@
         <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F28">
         <v>164</v>
@@ -1782,7 +1776,7 @@
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F29">
         <v>164</v>
@@ -1814,7 +1808,7 @@
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F30">
         <v>172</v>
@@ -1840,13 +1834,13 @@
         <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D31">
         <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F31">
         <v>180</v>
@@ -1872,13 +1866,13 @@
         <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D32">
         <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F32">
         <v>180</v>
@@ -1904,13 +1898,13 @@
         <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="D33">
         <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F33">
         <v>188</v>
@@ -1919,13 +1913,13 @@
         <v>200</v>
       </c>
       <c r="H33">
-        <v>323</v>
+        <v>188</v>
       </c>
       <c r="I33">
-        <v>335</v>
+        <v>200</v>
       </c>
       <c r="J33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1936,13 +1930,13 @@
         <v>91</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D34">
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F34">
         <v>188</v>
@@ -1951,13 +1945,13 @@
         <v>196</v>
       </c>
       <c r="H34">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I34">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="J34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1968,13 +1962,13 @@
         <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D35">
         <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F35">
         <v>188</v>
@@ -1983,10 +1977,10 @@
         <v>192</v>
       </c>
       <c r="H35">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="I35">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="J35" t="b">
         <v>0</v>
@@ -2000,25 +1994,25 @@
         <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D36">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F36">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="G36">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="H36">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="I36">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="J36" t="b">
         <v>1</v>
@@ -2029,28 +2023,28 @@
         <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="D37">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E37" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F37">
         <v>200</v>
       </c>
       <c r="G37">
+        <v>228</v>
+      </c>
+      <c r="H37">
+        <v>204</v>
+      </c>
+      <c r="I37">
         <v>232</v>
-      </c>
-      <c r="H37">
-        <v>335</v>
-      </c>
-      <c r="I37">
-        <v>335</v>
       </c>
       <c r="J37" t="b">
         <v>0</v>
@@ -2064,28 +2058,28 @@
         <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="D38">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E38" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F38">
-        <v>200</v>
+        <v>232</v>
       </c>
       <c r="G38">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="H38">
-        <v>335</v>
+        <v>232</v>
       </c>
       <c r="I38">
-        <v>335</v>
+        <v>250</v>
       </c>
       <c r="J38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2102,19 +2096,19 @@
         <v>18</v>
       </c>
       <c r="E39" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F39">
-        <v>214</v>
+        <v>250</v>
       </c>
       <c r="G39">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="H39">
-        <v>214</v>
+        <v>250</v>
       </c>
       <c r="I39">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="J39" t="b">
         <v>1</v>
@@ -2134,19 +2128,19 @@
         <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F40">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="G40">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="H40">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="I40">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="J40" t="b">
         <v>1</v>
@@ -2166,19 +2160,19 @@
         <v>16</v>
       </c>
       <c r="E41" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F41">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="G41">
-        <v>248</v>
+        <v>284</v>
       </c>
       <c r="H41">
-        <v>244</v>
+        <v>280</v>
       </c>
       <c r="I41">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="J41" t="b">
         <v>0</v>
@@ -2198,19 +2192,19 @@
         <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F42">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="G42">
-        <v>240</v>
+        <v>276</v>
       </c>
       <c r="H42">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="I42">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="J42" t="b">
         <v>0</v>
@@ -2230,19 +2224,19 @@
         <v>4</v>
       </c>
       <c r="E43" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F43">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="G43">
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="H43">
-        <v>256</v>
+        <v>292</v>
       </c>
       <c r="I43">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="J43" t="b">
         <v>0</v>
@@ -2262,19 +2256,19 @@
         <v>4</v>
       </c>
       <c r="E44" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F44">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="G44">
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="H44">
-        <v>256</v>
+        <v>292</v>
       </c>
       <c r="I44">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="J44" t="b">
         <v>0</v>
@@ -2294,19 +2288,19 @@
         <v>16</v>
       </c>
       <c r="E45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F45">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="G45">
-        <v>248</v>
+        <v>284</v>
       </c>
       <c r="H45">
-        <v>244</v>
+        <v>280</v>
       </c>
       <c r="I45">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="J45" t="b">
         <v>0</v>
@@ -2326,19 +2320,19 @@
         <v>24</v>
       </c>
       <c r="E46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F46">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="G46">
-        <v>256</v>
+        <v>292</v>
       </c>
       <c r="H46">
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="I46">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="J46" t="b">
         <v>0</v>
@@ -2358,19 +2352,19 @@
         <v>6</v>
       </c>
       <c r="E47" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F47">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="G47">
-        <v>266</v>
+        <v>302</v>
       </c>
       <c r="H47">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="I47">
-        <v>266</v>
+        <v>302</v>
       </c>
       <c r="J47" t="b">
         <v>1</v>
@@ -2390,19 +2384,19 @@
         <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F48">
-        <v>266</v>
+        <v>302</v>
       </c>
       <c r="G48">
-        <v>278</v>
+        <v>314</v>
       </c>
       <c r="H48">
-        <v>266</v>
+        <v>302</v>
       </c>
       <c r="I48">
-        <v>278</v>
+        <v>314</v>
       </c>
       <c r="J48" t="b">
         <v>1</v>
@@ -2422,19 +2416,19 @@
         <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F49">
-        <v>266</v>
+        <v>302</v>
       </c>
       <c r="G49">
-        <v>274</v>
+        <v>310</v>
       </c>
       <c r="H49">
-        <v>270</v>
+        <v>306</v>
       </c>
       <c r="I49">
-        <v>278</v>
+        <v>314</v>
       </c>
       <c r="J49" t="b">
         <v>0</v>
@@ -2454,19 +2448,19 @@
         <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F50">
-        <v>266</v>
+        <v>302</v>
       </c>
       <c r="G50">
-        <v>272</v>
+        <v>308</v>
       </c>
       <c r="H50">
-        <v>272</v>
+        <v>308</v>
       </c>
       <c r="I50">
-        <v>278</v>
+        <v>314</v>
       </c>
       <c r="J50" t="b">
         <v>0</v>
@@ -2486,19 +2480,19 @@
         <v>8</v>
       </c>
       <c r="E51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F51">
-        <v>278</v>
+        <v>314</v>
       </c>
       <c r="G51">
-        <v>286</v>
+        <v>322</v>
       </c>
       <c r="H51">
-        <v>278</v>
+        <v>314</v>
       </c>
       <c r="I51">
-        <v>286</v>
+        <v>322</v>
       </c>
       <c r="J51" t="b">
         <v>1</v>
@@ -2518,19 +2512,19 @@
         <v>18</v>
       </c>
       <c r="E52" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F52">
-        <v>286</v>
+        <v>322</v>
       </c>
       <c r="G52">
-        <v>304</v>
+        <v>340</v>
       </c>
       <c r="H52">
-        <v>286</v>
+        <v>322</v>
       </c>
       <c r="I52">
-        <v>304</v>
+        <v>340</v>
       </c>
       <c r="J52" t="b">
         <v>1</v>
@@ -2550,19 +2544,19 @@
         <v>4</v>
       </c>
       <c r="E53" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F53">
-        <v>304</v>
+        <v>340</v>
       </c>
       <c r="G53">
-        <v>308</v>
+        <v>344</v>
       </c>
       <c r="H53">
-        <v>312</v>
+        <v>348</v>
       </c>
       <c r="I53">
-        <v>316</v>
+        <v>352</v>
       </c>
       <c r="J53" t="b">
         <v>0</v>
@@ -2582,19 +2576,19 @@
         <v>12</v>
       </c>
       <c r="E54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F54">
-        <v>304</v>
+        <v>340</v>
       </c>
       <c r="G54">
-        <v>316</v>
+        <v>352</v>
       </c>
       <c r="H54">
-        <v>304</v>
+        <v>340</v>
       </c>
       <c r="I54">
-        <v>316</v>
+        <v>352</v>
       </c>
       <c r="J54" t="b">
         <v>1</v>
@@ -2614,19 +2608,19 @@
         <v>4</v>
       </c>
       <c r="E55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F55">
-        <v>304</v>
+        <v>340</v>
       </c>
       <c r="G55">
-        <v>308</v>
+        <v>344</v>
       </c>
       <c r="H55">
-        <v>312</v>
+        <v>348</v>
       </c>
       <c r="I55">
-        <v>316</v>
+        <v>352</v>
       </c>
       <c r="J55" t="b">
         <v>0</v>
@@ -2646,19 +2640,19 @@
         <v>4</v>
       </c>
       <c r="E56" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F56">
-        <v>316</v>
+        <v>352</v>
       </c>
       <c r="G56">
-        <v>320</v>
+        <v>356</v>
       </c>
       <c r="H56">
-        <v>316</v>
+        <v>352</v>
       </c>
       <c r="I56">
-        <v>320</v>
+        <v>356</v>
       </c>
       <c r="J56" t="b">
         <v>1</v>
@@ -2678,19 +2672,19 @@
         <v>4</v>
       </c>
       <c r="E57" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F57">
-        <v>316</v>
+        <v>352</v>
       </c>
       <c r="G57">
-        <v>320</v>
+        <v>356</v>
       </c>
       <c r="H57">
-        <v>316</v>
+        <v>352</v>
       </c>
       <c r="I57">
-        <v>320</v>
+        <v>356</v>
       </c>
       <c r="J57" t="b">
         <v>1</v>
@@ -2710,19 +2704,19 @@
         <v>4</v>
       </c>
       <c r="E58" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F58">
-        <v>320</v>
+        <v>356</v>
       </c>
       <c r="G58">
-        <v>324</v>
+        <v>360</v>
       </c>
       <c r="H58">
-        <v>322</v>
+        <v>358</v>
       </c>
       <c r="I58">
-        <v>326</v>
+        <v>362</v>
       </c>
       <c r="J58" t="b">
         <v>0</v>
@@ -2742,19 +2736,19 @@
         <v>6</v>
       </c>
       <c r="E59" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F59">
-        <v>320</v>
+        <v>356</v>
       </c>
       <c r="G59">
-        <v>326</v>
+        <v>362</v>
       </c>
       <c r="H59">
-        <v>320</v>
+        <v>356</v>
       </c>
       <c r="I59">
-        <v>326</v>
+        <v>362</v>
       </c>
       <c r="J59" t="b">
         <v>1</v>
@@ -2774,19 +2768,19 @@
         <v>4</v>
       </c>
       <c r="E60" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F60">
-        <v>320</v>
+        <v>356</v>
       </c>
       <c r="G60">
-        <v>324</v>
+        <v>360</v>
       </c>
       <c r="H60">
-        <v>322</v>
+        <v>358</v>
       </c>
       <c r="I60">
-        <v>326</v>
+        <v>362</v>
       </c>
       <c r="J60" t="b">
         <v>0</v>
@@ -2806,19 +2800,19 @@
         <v>4</v>
       </c>
       <c r="E61" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F61">
-        <v>326</v>
+        <v>362</v>
       </c>
       <c r="G61">
-        <v>330</v>
+        <v>366</v>
       </c>
       <c r="H61">
-        <v>326</v>
+        <v>362</v>
       </c>
       <c r="I61">
-        <v>330</v>
+        <v>366</v>
       </c>
       <c r="J61" t="b">
         <v>1</v>
@@ -2838,19 +2832,19 @@
         <v>4</v>
       </c>
       <c r="E62" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F62">
-        <v>330</v>
+        <v>366</v>
       </c>
       <c r="G62">
-        <v>334</v>
+        <v>370</v>
       </c>
       <c r="H62">
-        <v>330</v>
+        <v>366</v>
       </c>
       <c r="I62">
-        <v>334</v>
+        <v>370</v>
       </c>
       <c r="J62" t="b">
         <v>1</v>
@@ -2864,25 +2858,25 @@
         <v>105</v>
       </c>
       <c r="C63" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F63">
-        <v>334</v>
+        <v>370</v>
       </c>
       <c r="G63">
-        <v>335</v>
+        <v>371</v>
       </c>
       <c r="H63">
-        <v>334</v>
+        <v>370</v>
       </c>
       <c r="I63">
-        <v>335</v>
+        <v>371</v>
       </c>
       <c r="J63" t="b">
         <v>1</v>
@@ -2902,16 +2896,16 @@
         <v>0</v>
       </c>
       <c r="F64">
-        <v>335</v>
+        <v>371</v>
       </c>
       <c r="G64">
-        <v>335</v>
+        <v>371</v>
       </c>
       <c r="H64">
-        <v>335</v>
+        <v>371</v>
       </c>
       <c r="I64">
-        <v>335</v>
+        <v>371</v>
       </c>
       <c r="J64" t="b">
         <v>1</v>

</xml_diff>